<commit_message>
success : add student and get student endpoint
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1233EF94-D11D-435B-8026-E36F038771B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="20000" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="student" state="visible" r:id="rId4"/>
+    <sheet name="student" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -25,26 +26,68 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Charlie</t>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>aktif</t>
+  </si>
+  <si>
+    <t>nonaktif</t>
+  </si>
+  <si>
+    <t>lulus</t>
+  </si>
+  <si>
+    <t>alumni</t>
+  </si>
+  <si>
+    <t>Emma Smith</t>
+  </si>
+  <si>
+    <t>Liam Johnson</t>
+  </si>
+  <si>
+    <t>Olivia Williams</t>
+  </si>
+  <si>
+    <t>Noa Brown</t>
+  </si>
+  <si>
+    <t>Aiden Jones</t>
+  </si>
+  <si>
+    <t>Amelia Miller</t>
+  </si>
+  <si>
+    <t>Ethan Davis</t>
+  </si>
+  <si>
+    <t>Charlotte Garcia</t>
+  </si>
+  <si>
+    <t>Harper Rodriguez</t>
+  </si>
+  <si>
+    <t>Mason Wilson</t>
+  </si>
+  <si>
+    <t>Scarlett Moore</t>
+  </si>
+  <si>
+    <t>Logan Taylor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -407,11 +450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,42 +472,180 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
         <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>